<commit_message>
added a test tex file
</commit_message>
<xml_diff>
--- a/budget.xlsx
+++ b/budget.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEE6A95-DC42-47F4-B576-EF26AB61D6DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01749CD8-DEF8-4815-B52E-1C30101FD62D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,34 +15,24 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Composant</t>
   </si>
   <si>
-    <t>Coût</t>
-  </si>
-  <si>
-    <t>Arduino Leonardo</t>
-  </si>
-  <si>
-    <t>https://www.amazon.fr/MagiDeal-Leonardo-ATmega32U4-Arduino-Compatible/dp/B06ZYVQ2T3/ref=sr_1_9?ie=UTF8&amp;qid=1536697174&amp;sr=8-9&amp;keywords=arduino+leonardo</t>
-  </si>
-  <si>
-    <t>Lien</t>
-  </si>
-  <si>
     <t>Ecran LCD Tactile</t>
   </si>
   <si>
-    <t>https://www.amazon.fr/ELEGOO-Tactile-320x240-Technical-Arduino/dp/B01JD4TJZU/ref=sr_1_1_sspa?ie=UTF8&amp;qid=1536706267&amp;sr=8-1-spons&amp;keywords=arduino+lcd+touch+screen&amp;psc=1</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -52,17 +42,25 @@
     <t>Boitier bas</t>
   </si>
   <si>
-    <t>voir OnShape</t>
+    <t>Arduino Zero</t>
+  </si>
+  <si>
+    <t>Coût ($)</t>
+  </si>
+  <si>
+    <t>Coût (€)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +91,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,19 +117,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -406,79 +418,69 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="20.578125" customWidth="1"/>
-    <col min="3" max="3" width="10.47265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.41796875" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.47265625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="4" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:4" s="2" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8.11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>12.72</v>
+      </c>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.36</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
         <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
+    </row>
+    <row r="9" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5">
         <f>SUM(C3:C8)</f>
-        <v>25.099999999999998</v>
-      </c>
+        <v>18.080000000000002</v>
+      </c>
+      <c r="D9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>